<commit_message>
modified datatypes; added new attributes
</commit_message>
<xml_diff>
--- a/dist/rd3_portal.xlsx
+++ b/dist/rd3_portal.xlsx
@@ -16,12 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
   <si>
     <t>rd3_portal</t>
   </si>
   <si>
-    <t>cluster</t>
+    <t>rd3_portal_cluster</t>
   </si>
   <si>
     <t>RD3 Portal Data</t>
@@ -33,7 +33,7 @@
     <t>RD3 portal, containing data submitted by CNAG (v1.1.0, 2021-10-11)</t>
   </si>
   <si>
-    <t>Extracted metadata PED and Phenopacket files stored on the cluster (v0.9.0, 2022-08-01)</t>
+    <t>Extracted metadata PED and Phenopacket files stored on the cluster (v0.9.1, 2022-08-01)</t>
   </si>
   <si>
     <t>phenopacket</t>
@@ -45,7 +45,7 @@
     <t>Extracted data from Phenopacket files</t>
   </si>
   <si>
-    <t>cluster_phenopacket</t>
+    <t>rd3_portal_cluster_phenopacket</t>
   </si>
   <si>
     <t>phenopacketsID</t>
@@ -72,7 +72,10 @@
     <t>ageOfOnset</t>
   </si>
   <si>
-    <t>subjectIdExists</t>
+    <t>subjectExists</t>
+  </si>
+  <si>
+    <t>releasesWhereSubjectExists</t>
   </si>
   <si>
     <t>unknownHpoCodes</t>
@@ -84,6 +87,9 @@
     <t>unknownOnsetCodes</t>
   </si>
   <si>
+    <t>processed</t>
+  </si>
+  <si>
     <t>Name of the Phenopacket file</t>
   </si>
   <si>
@@ -108,6 +114,9 @@
     <t>An indication if the subject exists in RD3</t>
   </si>
   <si>
+    <t>If the subject exists, which release</t>
+  </si>
+  <si>
     <t>A comma-separated string of all unknown HPO codes</t>
   </si>
   <si>
@@ -117,9 +126,15 @@
     <t>A comma-separated string of all unknown onset codes</t>
   </si>
   <si>
+    <t>An indication if the data has been imported into RD3 somewhere</t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
+    <t>text</t>
+  </si>
+  <si>
     <t>bool</t>
   </si>
   <si>
@@ -130,6 +145,9 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>parent</t>
   </si>
   <si>
     <t>package</t>
@@ -500,24 +518,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -528,7 +549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -537,6 +558,9 @@
       </c>
       <c r="C3" t="s">
         <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -554,16 +578,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -587,7 +611,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -595,31 +619,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -630,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -639,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G2" t="b">
         <v>1</v>
@@ -656,10 +680,10 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G3" t="b">
         <v>1</v>
@@ -676,10 +700,10 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
@@ -696,10 +720,10 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G5" t="b">
         <v>1</v>
@@ -716,10 +740,10 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G6" t="b">
         <v>1</v>
@@ -736,10 +760,10 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G7" t="b">
         <v>1</v>
@@ -756,10 +780,10 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G8" t="b">
         <v>1</v>
@@ -776,10 +800,10 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G9" t="b">
         <v>1</v>
@@ -796,10 +820,10 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G10" t="b">
         <v>1</v>
@@ -819,10 +843,10 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G11" t="b">
         <v>1</v>
@@ -839,10 +863,10 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G12" t="b">
         <v>1</v>
@@ -859,15 +883,58 @@
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="G13" t="b">
         <v>1</v>
       </c>
       <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
init emx for raw ped data
</commit_message>
<xml_diff>
--- a/dist/rd3_portal.xlsx
+++ b/dist/rd3_portal.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="80">
   <si>
     <t>rd3_portal</t>
   </si>
@@ -33,21 +33,33 @@
     <t>RD3 portal, containing data submitted by CNAG (v1.1.0, 2021-10-11)</t>
   </si>
   <si>
-    <t>Extracted metadata PED and Phenopacket files stored on the cluster (v0.9.2, 2022-08-02)</t>
+    <t>Extracted metadata PED and Phenopacket files stored on the cluster (v1.0.0, 2022-08-08)</t>
   </si>
   <si>
     <t>phenopacket</t>
   </si>
   <si>
+    <t>ped</t>
+  </si>
+  <si>
     <t>Phenopacket</t>
   </si>
   <si>
+    <t>PED</t>
+  </si>
+  <si>
     <t>Extracted data from Phenopacket files</t>
   </si>
   <si>
+    <t>Extracted data from PED files</t>
+  </si>
+  <si>
     <t>rd3_portal_cluster_phenopacket</t>
   </si>
   <si>
+    <t>rd3_portal_cluster_ped</t>
+  </si>
+  <si>
     <t>phenopacketsID</t>
   </si>
   <si>
@@ -93,6 +105,39 @@
     <t>processed</t>
   </si>
   <si>
+    <t>rowID</t>
+  </si>
+  <si>
+    <t>pedID</t>
+  </si>
+  <si>
+    <t>fid</t>
+  </si>
+  <si>
+    <t>mid</t>
+  </si>
+  <si>
+    <t>pid</t>
+  </si>
+  <si>
+    <t>clinical_status</t>
+  </si>
+  <si>
+    <t>unknownMID</t>
+  </si>
+  <si>
+    <t>unknownPID</t>
+  </si>
+  <si>
+    <t>unknownSexCodes</t>
+  </si>
+  <si>
+    <t>unknownClinicalStatus</t>
+  </si>
+  <si>
+    <t>upload</t>
+  </si>
+  <si>
     <t>Name of the Phenopacket file</t>
   </si>
   <si>
@@ -135,6 +180,36 @@
     <t>An indication if the data has been imported into RD3 somewhere</t>
   </si>
   <si>
+    <t>an auto generated ID</t>
+  </si>
+  <si>
+    <t>family identifier</t>
+  </si>
+  <si>
+    <t>identifier of the mother</t>
+  </si>
+  <si>
+    <t>identifier of the father</t>
+  </si>
+  <si>
+    <t>An indication of affected status</t>
+  </si>
+  <si>
+    <t>The identifier of the mother that was reported. It was either invalid or could not be found in RD3</t>
+  </si>
+  <si>
+    <t>The identifier of the father that was reported. It was either invalid or could not be found in RD3</t>
+  </si>
+  <si>
+    <t>Code that was detected in the PED file, but it does not match expected values (1,2, other)</t>
+  </si>
+  <si>
+    <t>A code that was detected in the PED file, but it does not match an expected value (-9, 0, 1,2)</t>
+  </si>
+  <si>
+    <t>If True, the raw data for this subject can be imported into RD3</t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
@@ -178,6 +253,9 @@
   </si>
   <si>
     <t>defaultValue</t>
+  </si>
+  <si>
+    <t>auto</t>
   </si>
 </sst>
 </file>
@@ -532,16 +610,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -576,7 +654,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -584,16 +662,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -604,10 +682,24 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -617,350 +709,708 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" t="s">
+        <v>64</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" t="b">
-        <v>1</v>
-      </c>
-      <c r="H9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" t="b">
-        <v>1</v>
-      </c>
-      <c r="H14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" t="b">
+      <c r="F33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="b">
+        <v>0</v>
+      </c>
+      <c r="I33" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new portal table
</commit_message>
<xml_diff>
--- a/dist/rd3_portal.xlsx
+++ b/dist/rd3_portal.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
   <si>
     <t>rd3_portal</t>
   </si>
@@ -42,13 +42,22 @@
     <t>patches</t>
   </si>
   <si>
+    <t>new</t>
+  </si>
+  <si>
     <t>All patches</t>
   </si>
   <si>
+    <t>New Metadata</t>
+  </si>
+  <si>
     <t>Attribute template for new RD3 Data Freezes</t>
   </si>
   <si>
     <t>Staging table for all patches</t>
+  </si>
+  <si>
+    <t>New metadata that was found in the "All patches" table</t>
   </si>
   <si>
     <t>rd3_portal_release_attrTmplate</t>
@@ -592,16 +601,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -636,7 +645,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -644,22 +653,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -673,7 +682,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -687,13 +696,30 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -711,42 +737,42 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -760,16 +786,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -783,16 +809,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -806,16 +832,16 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -829,16 +855,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -852,16 +878,16 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -875,16 +901,16 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -898,16 +924,16 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -921,16 +947,16 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -944,16 +970,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -967,16 +993,16 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -990,16 +1016,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1013,16 +1039,16 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1036,16 +1062,16 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1059,16 +1085,16 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1082,16 +1108,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1105,16 +1131,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1128,16 +1154,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -1151,16 +1177,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1174,16 +1200,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1197,16 +1223,16 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1220,16 +1246,16 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1243,16 +1269,16 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1266,16 +1292,16 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
added new release table for experiments
</commit_message>
<xml_diff>
--- a/dist/rd3_portal.xlsx
+++ b/dist/rd3_portal.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="131">
   <si>
     <t>rd3_portal</t>
   </si>
@@ -33,36 +33,54 @@
     <t>RD3 portal, containing data submitted by CNAG (v1.2.0, 2022-11-29)</t>
   </si>
   <si>
-    <t>Intermediate tables for RD3 releases (v1.2.0, 2023-01-25)</t>
+    <t>Intermediate tables for RD3 releases (v1.3.0, 2023-04-05)</t>
   </si>
   <si>
     <t>attrTmplate</t>
   </si>
   <si>
+    <t>exprTemplate</t>
+  </si>
+  <si>
     <t>patches</t>
   </si>
   <si>
     <t>new</t>
   </si>
   <si>
+    <t>experiments</t>
+  </si>
+  <si>
     <t>All patches</t>
   </si>
   <si>
     <t>New Metadata</t>
   </si>
   <si>
+    <t>Experiments</t>
+  </si>
+  <si>
     <t>Attribute template for new RD3 Data Freezes</t>
   </si>
   <si>
+    <t>template for experiments</t>
+  </si>
+  <si>
     <t>Staging table for all patches</t>
   </si>
   <si>
     <t>New metadata that was found in the "All patches" table</t>
   </si>
   <si>
+    <t>Staging table for experiment metadata</t>
+  </si>
+  <si>
     <t>rd3_portal_release_attrTmplate</t>
   </si>
   <si>
+    <t>rd3_portal_release_exprTemplate</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -135,6 +153,138 @@
     <t>processed</t>
   </si>
   <si>
+    <t>file_path</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>unencrypted_md5_checksum</t>
+  </si>
+  <si>
+    <t>encrypted_md5_checksum</t>
+  </si>
+  <si>
+    <t>file_type</t>
+  </si>
+  <si>
+    <t>file_size</t>
+  </si>
+  <si>
+    <t>file_group_id</t>
+  </si>
+  <si>
+    <t>batch_id</t>
+  </si>
+  <si>
+    <t>project_experiment_dataset_id</t>
+  </si>
+  <si>
+    <t>sample_id</t>
+  </si>
+  <si>
+    <t>sample_links</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>phenotype</t>
+  </si>
+  <si>
+    <t>subject_links</t>
+  </si>
+  <si>
+    <t>sequencing_center</t>
+  </si>
+  <si>
+    <t>platform_brand</t>
+  </si>
+  <si>
+    <t>platform_model</t>
+  </si>
+  <si>
+    <t>library_source</t>
+  </si>
+  <si>
+    <t>library_selection</t>
+  </si>
+  <si>
+    <t>library_strategy</t>
+  </si>
+  <si>
+    <t>library_layout</t>
+  </si>
+  <si>
+    <t>paired_nominal_length</t>
+  </si>
+  <si>
+    <t>paired_nominal_sdev</t>
+  </si>
+  <si>
+    <t>experiment_links</t>
+  </si>
+  <si>
+    <t>analysis_center</t>
+  </si>
+  <si>
+    <t>analysis_type</t>
+  </si>
+  <si>
+    <t>sequencing_type</t>
+  </si>
+  <si>
+    <t>reference_genome</t>
+  </si>
+  <si>
+    <t>linked_object</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>program</t>
+  </si>
+  <si>
+    <t>imputation</t>
+  </si>
+  <si>
+    <t>analysis_links</t>
+  </si>
+  <si>
+    <t>experiment_type</t>
+  </si>
+  <si>
+    <t>tissue_type</t>
+  </si>
+  <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>sub_project_name</t>
+  </si>
+  <si>
+    <t>project_batch_id</t>
+  </si>
+  <si>
+    <t>file_ega_id</t>
+  </si>
+  <si>
+    <t>run_ega_id</t>
+  </si>
+  <si>
+    <t>experiment_ega_id</t>
+  </si>
+  <si>
+    <t>sample_ega_id</t>
+  </si>
+  <si>
+    <t>date_created</t>
+  </si>
+  <si>
+    <t>molgenis_id</t>
+  </si>
+  <si>
     <t>auto generated molgenis ID</t>
   </si>
   <si>
@@ -204,10 +354,22 @@
     <t>If True, the record has been processed</t>
   </si>
   <si>
+    <t>Date the data was uploaded into RD3</t>
+  </si>
+  <si>
+    <t>indication if the the record has been processed into an RD3 release</t>
+  </si>
+  <si>
+    <t>an internal, auto generated identifier</t>
+  </si>
+  <si>
     <t>string</t>
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>datetime</t>
   </si>
   <si>
     <t>name</t>
@@ -601,16 +763,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -645,7 +807,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -653,22 +815,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -682,7 +844,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -695,14 +857,11 @@
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -713,13 +872,47 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
-        <v>14</v>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -729,7 +922,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -737,42 +930,42 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>118</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>72</v>
+        <v>126</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>73</v>
+        <v>127</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>74</v>
+        <v>128</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>76</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -786,16 +979,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -809,16 +1002,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -832,16 +1025,16 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -855,16 +1048,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -878,16 +1071,16 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -901,16 +1094,16 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -924,16 +1117,16 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -947,16 +1140,16 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -970,16 +1163,16 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="D11" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -993,16 +1186,16 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1016,16 +1209,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1039,16 +1232,16 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1062,16 +1255,16 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="D15" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1085,16 +1278,16 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1108,16 +1301,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1131,16 +1324,16 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1154,16 +1347,16 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -1177,16 +1370,16 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1200,16 +1393,16 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1223,16 +1416,16 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1246,16 +1439,16 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1269,16 +1462,16 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1292,27 +1485,959 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E38" t="b">
+        <v>0</v>
+      </c>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39" t="s">
+        <v>115</v>
+      </c>
+      <c r="E39" t="b">
+        <v>0</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" t="s">
+        <v>115</v>
+      </c>
+      <c r="E40" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" t="s">
+        <v>115</v>
+      </c>
+      <c r="E41" t="b">
+        <v>0</v>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" t="s">
         <v>61</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D43" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" t="b">
+        <v>0</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" t="s">
         <v>63</v>
       </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G25" t="b">
-        <v>1</v>
-      </c>
-      <c r="H25" t="b">
+      <c r="D45" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="D46" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" t="s">
+        <v>115</v>
+      </c>
+      <c r="E47" t="b">
+        <v>0</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="s">
+        <v>66</v>
+      </c>
+      <c r="D48" t="s">
+        <v>115</v>
+      </c>
+      <c r="E48" t="b">
+        <v>0</v>
+      </c>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" t="s">
+        <v>115</v>
+      </c>
+      <c r="E49" t="b">
+        <v>0</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" t="s">
+        <v>68</v>
+      </c>
+      <c r="D50" t="s">
+        <v>115</v>
+      </c>
+      <c r="E50" t="b">
+        <v>0</v>
+      </c>
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" t="s">
+        <v>115</v>
+      </c>
+      <c r="E51" t="b">
+        <v>0</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" t="s">
+        <v>115</v>
+      </c>
+      <c r="E52" t="b">
+        <v>0</v>
+      </c>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>20</v>
+      </c>
+      <c r="B53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" t="s">
+        <v>115</v>
+      </c>
+      <c r="E53" t="b">
+        <v>0</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>20</v>
+      </c>
+      <c r="B54" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E54" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" t="s">
+        <v>115</v>
+      </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>20</v>
+      </c>
+      <c r="B56" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" t="s">
+        <v>115</v>
+      </c>
+      <c r="E56" t="b">
+        <v>0</v>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" t="s">
+        <v>75</v>
+      </c>
+      <c r="D57" t="s">
+        <v>115</v>
+      </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>20</v>
+      </c>
+      <c r="B58" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" t="s">
+        <v>115</v>
+      </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" t="s">
+        <v>115</v>
+      </c>
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" t="s">
+        <v>115</v>
+      </c>
+      <c r="E60" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>79</v>
+      </c>
+      <c r="D61" t="s">
+        <v>115</v>
+      </c>
+      <c r="E61" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="G61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>80</v>
+      </c>
+      <c r="D62" t="s">
+        <v>115</v>
+      </c>
+      <c r="E62" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" t="s">
+        <v>115</v>
+      </c>
+      <c r="E63" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64" t="s">
+        <v>115</v>
+      </c>
+      <c r="E64" t="b">
+        <v>0</v>
+      </c>
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+      <c r="G64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" t="s">
+        <v>83</v>
+      </c>
+      <c r="D65" t="s">
+        <v>115</v>
+      </c>
+      <c r="E65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" t="b">
+        <v>0</v>
+      </c>
+      <c r="G65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" t="s">
+        <v>84</v>
+      </c>
+      <c r="D66" t="s">
+        <v>115</v>
+      </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="G66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" t="s">
+        <v>85</v>
+      </c>
+      <c r="D67" t="s">
+        <v>115</v>
+      </c>
+      <c r="E67" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" t="s">
+        <v>86</v>
+      </c>
+      <c r="D68" t="s">
+        <v>115</v>
+      </c>
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" t="s">
+        <v>87</v>
+      </c>
+      <c r="C69" t="s">
+        <v>112</v>
+      </c>
+      <c r="D69" t="s">
+        <v>117</v>
+      </c>
+      <c r="E69" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" t="b">
+        <v>1</v>
+      </c>
+      <c r="G69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" t="s">
+        <v>44</v>
+      </c>
+      <c r="C70" t="s">
+        <v>113</v>
+      </c>
+      <c r="D70" t="s">
+        <v>116</v>
+      </c>
+      <c r="E70" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+      <c r="G70" t="b">
+        <v>1</v>
+      </c>
+      <c r="H70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="A71" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" t="s">
+        <v>114</v>
+      </c>
+      <c r="D71" t="s">
+        <v>115</v>
+      </c>
+      <c r="E71" t="b">
+        <v>1</v>
+      </c>
+      <c r="F71" t="b">
+        <v>1</v>
+      </c>
+      <c r="G71" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: model adjustments; new table for re-analysis
</commit_message>
<xml_diff>
--- a/dist/rd3_portal.xlsx
+++ b/dist/rd3_portal.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="134">
   <si>
     <t>name</t>
   </si>
@@ -33,76 +33,169 @@
     <t>rd3_portal</t>
   </si>
   <si>
-    <t>rd3_portal_novelomics</t>
+    <t>rd3_portal_release</t>
   </si>
   <si>
     <t>RD3 Portal Data</t>
   </si>
   <si>
-    <t>Novel Omics</t>
+    <t>Releases</t>
   </si>
   <si>
     <t>RD3 portal, containing data submitted by CNAG (v1.2.0, 2022-11-29)</t>
   </si>
   <si>
-    <t>Staging tables for novel omics sample and experiment metadata (v1.7.0, 2024-04-05)</t>
+    <t>Intermediate tables for RD3 releases (v1.4.0, 2024-04-23)</t>
   </si>
   <si>
     <t>package</t>
   </si>
   <si>
-    <t>experiment</t>
-  </si>
-  <si>
-    <t>shipment</t>
-  </si>
-  <si>
-    <t>datasets</t>
-  </si>
-  <si>
-    <t>Experiment</t>
-  </si>
-  <si>
-    <t>Shipment</t>
-  </si>
-  <si>
-    <t>Datasets</t>
-  </si>
-  <si>
-    <t>Staging table for experiment metadata (manifest file)</t>
-  </si>
-  <si>
-    <t>Staging table for sample metadata</t>
-  </si>
-  <si>
-    <t>Link between EGA datasets and runs/analyses</t>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>extends</t>
+  </si>
+  <si>
+    <t>attrTmplate</t>
+  </si>
+  <si>
+    <t>exprTemplate</t>
+  </si>
+  <si>
+    <t>patches</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>experiments</t>
+  </si>
+  <si>
+    <t>df1</t>
+  </si>
+  <si>
+    <t>All patches</t>
+  </si>
+  <si>
+    <t>New Metadata</t>
+  </si>
+  <si>
+    <t>Experiments</t>
+  </si>
+  <si>
+    <t>Data Freeze 1 Reanalysis</t>
+  </si>
+  <si>
+    <t>Attribute template for new RD3 Data Freezes</t>
+  </si>
+  <si>
+    <t>template for experiments</t>
+  </si>
+  <si>
+    <t>Staging table for all patches</t>
+  </si>
+  <si>
+    <t>New metadata that was found in the "All patches" table</t>
+  </si>
+  <si>
+    <t>Staging table for experiment metadata</t>
+  </si>
+  <si>
+    <t>rd3_portal_release_attrTmplate</t>
+  </si>
+  <si>
+    <t>rd3_portal_release_exprTemplate</t>
   </si>
   <si>
     <t>entity</t>
   </si>
   <si>
+    <t>dataType</t>
+  </si>
+  <si>
+    <t>idAttribute</t>
+  </si>
+  <si>
     <t>auto</t>
   </si>
   <si>
-    <t>dataType</t>
-  </si>
-  <si>
-    <t>idAttribute</t>
-  </si>
-  <si>
     <t>nillable</t>
   </si>
   <si>
     <t>defaultValue</t>
   </si>
   <si>
-    <t>rd3_portal_novelomics_experiment</t>
-  </si>
-  <si>
-    <t>rd3_portal_novelomics_shipment</t>
-  </si>
-  <si>
-    <t>rd3_portal_novelomics_datasets</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>organisation_name</t>
+  </si>
+  <si>
+    <t>organisation_identifier</t>
+  </si>
+  <si>
+    <t>samples_tissueType</t>
+  </si>
+  <si>
+    <t>samples_id</t>
+  </si>
+  <si>
+    <t>samples_alternativeIdentifier</t>
+  </si>
+  <si>
+    <t>samples_subject</t>
+  </si>
+  <si>
+    <t>samples_organisation</t>
+  </si>
+  <si>
+    <t>samples_ERN</t>
+  </si>
+  <si>
+    <t>labinfo_library</t>
+  </si>
+  <si>
+    <t>labinfo_sequencer</t>
+  </si>
+  <si>
+    <t>labinfo_seqType</t>
+  </si>
+  <si>
+    <t>labinfo_id</t>
+  </si>
+  <si>
+    <t>labinfo_sample</t>
+  </si>
+  <si>
+    <t>labinfo_capture</t>
+  </si>
+  <si>
+    <t>labinfo_libraryType</t>
+  </si>
+  <si>
+    <t>subject_id</t>
+  </si>
+  <si>
+    <t>subject_organisation</t>
+  </si>
+  <si>
+    <t>subject_ERN</t>
+  </si>
+  <si>
+    <t>subject_solved</t>
+  </si>
+  <si>
+    <t>subject_date_solved</t>
+  </si>
+  <si>
+    <t>subject_matchMakerPermission</t>
+  </si>
+  <si>
+    <t>subject_recontact</t>
+  </si>
+  <si>
+    <t>processed</t>
   </si>
   <si>
     <t>file_path</t>
@@ -141,9 +234,6 @@
     <t>gender</t>
   </si>
   <si>
-    <t>subject_id</t>
-  </si>
-  <si>
     <t>phenotype</t>
   </si>
   <si>
@@ -240,94 +330,94 @@
     <t>date_created</t>
   </si>
   <si>
-    <t>processed</t>
-  </si>
-  <si>
     <t>molgenis_id</t>
   </si>
   <si>
-    <t>participant_subject</t>
-  </si>
-  <si>
-    <t>type_of_analysis</t>
-  </si>
-  <si>
-    <t>solve_rd_experiment_id</t>
-  </si>
-  <si>
-    <t>batch</t>
-  </si>
-  <si>
-    <t>organisation</t>
+    <t>auto generated molgenis ID</t>
+  </si>
+  <si>
+    <t>name of the organisation. E.g. University Medical Center Groningen</t>
+  </si>
+  <si>
+    <t>identifier of the organisation. E.g. UMCG¬†</t>
+  </si>
+  <si>
+    <t>Tissue Types</t>
+  </si>
+  <si>
+    <t>unique identifier (sampleID + patch)</t>
+  </si>
+  <si>
+    <t>alternative identifier used by sample provider</t>
+  </si>
+  <si>
+    <t>reference to the subject from which samples was extracted</t>
+  </si>
+  <si>
+    <t>Name of the organisation. E.g. University Medical Center Groningen</t>
   </si>
   <si>
     <t>ERN</t>
   </si>
   <si>
-    <t>CNAG_barcode</t>
-  </si>
-  <si>
-    <t>alternative_sample_identifier</t>
-  </si>
-  <si>
-    <t>pathological_state</t>
-  </si>
-  <si>
-    <t>tumor_cell_fraction</t>
-  </si>
-  <si>
-    <t>anatomical_location</t>
-  </si>
-  <si>
-    <t>extracted_protocol</t>
-  </si>
-  <si>
-    <t>data_ega_id</t>
-  </si>
-  <si>
-    <t>run_or_analysis_ega_id</t>
-  </si>
-  <si>
-    <t>reference_type</t>
+    <t>link to more information about the library used in experiment</t>
+  </si>
+  <si>
+    <t>sequencer info</t>
+  </si>
+  <si>
+    <t>sequencing technique types (e.g., WGS, WXS)</t>
+  </si>
+  <si>
+    <t>Unique identifier (experimentID + patch)</t>
+  </si>
+  <si>
+    <t>all samples run in this condition, using the same barcode</t>
+  </si>
+  <si>
+    <t>enrichment kit</t>
+  </si>
+  <si>
+    <t>library source, e.g., Genomic/Transcriptomic</t>
+  </si>
+  <si>
+    <t>Unique identifier (subjectID + patch)</t>
+  </si>
+  <si>
+    <t>name of the organisation that submitted the subject</t>
+  </si>
+  <si>
+    <t>solved case for solve-RD (true/false)</t>
+  </si>
+  <si>
+    <t>Date case was solved</t>
+  </si>
+  <si>
+    <t>permission is given for match making (boolean)</t>
+  </si>
+  <si>
+    <t>Recontact is allowed in case of incidental findings</t>
+  </si>
+  <si>
+    <t>If True, the record has been processed</t>
+  </si>
+  <si>
+    <t>Date the data was uploaded into RD3</t>
+  </si>
+  <si>
+    <t>indication if the the record has been processed into an RD3 release</t>
+  </si>
+  <si>
+    <t>an internal, auto generated identifier</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
+    <t>bool</t>
+  </si>
+  <si>
     <t>datetime</t>
-  </si>
-  <si>
-    <t>bool</t>
-  </si>
-  <si>
-    <t>Date the data was uploaded into RD3</t>
-  </si>
-  <si>
-    <t>indication if the the record has been processed into an RD3 release</t>
-  </si>
-  <si>
-    <t>an internal, auto generated identifier</t>
-  </si>
-  <si>
-    <t>The analysis that was performed; e.g., SR-WGS, Deep-WES, RNAseq, etc.</t>
-  </si>
-  <si>
-    <t>corresponding experiment identifier</t>
-  </si>
-  <si>
-    <t>the submitting institution and submitter initials</t>
-  </si>
-  <si>
-    <t>associated ERN</t>
-  </si>
-  <si>
-    <t>alternative identifiers associated with the sample</t>
-  </si>
-  <si>
-    <t>affected state of the material</t>
-  </si>
-  <si>
-    <t>the percentange of tumor cells compared to total cells present in this material</t>
   </si>
 </sst>
 </file>
@@ -737,13 +827,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -756,47 +846,107 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>23</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>24</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -814,1447 +964,1477 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="b">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
       <c r="F3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
       <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
       <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
       </c>
       <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" t="b">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
       <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
       <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="b">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>112</v>
       </c>
       <c r="D9" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
       <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="b">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>113</v>
       </c>
       <c r="D10" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
       <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" t="b">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
       <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" t="b">
-        <v>0</v>
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>115</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
       <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="b">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>116</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
       <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="b">
-        <v>0</v>
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>117</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
       <c r="F14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" t="b">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>118</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
       <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="b">
-        <v>0</v>
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>119</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
       </c>
       <c r="F16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" t="b">
-        <v>0</v>
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
       <c r="F17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="b">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
       </c>
       <c r="F18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="b">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>122</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
       <c r="F19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" t="b">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
       </c>
       <c r="D20" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
       </c>
       <c r="F20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="b">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>123</v>
       </c>
       <c r="D21" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
       </c>
       <c r="F21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="b">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>124</v>
       </c>
       <c r="D22" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
       </c>
       <c r="F22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" t="b">
-        <v>0</v>
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>125</v>
       </c>
       <c r="D23" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
       </c>
       <c r="F23" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" t="b">
-        <v>0</v>
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>126</v>
       </c>
       <c r="D24" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
       </c>
       <c r="F24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>0</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" t="b">
+        <v>0</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" t="b">
+        <v>0</v>
+      </c>
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" t="b">
+        <v>0</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" t="b">
+        <v>0</v>
+      </c>
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" t="b">
+        <v>0</v>
+      </c>
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
+        <v>131</v>
+      </c>
+      <c r="E33" t="b">
+        <v>0</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" t="b">
+        <v>0</v>
+      </c>
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E35" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" t="b">
+        <v>0</v>
+      </c>
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" t="b">
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>29</v>
+      </c>
+      <c r="B38" t="s">
         <v>52</v>
       </c>
-      <c r="C25" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" t="s">
-        <v>91</v>
-      </c>
-      <c r="E25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" t="b">
-        <v>0</v>
-      </c>
-      <c r="F26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" t="b">
-        <v>0</v>
-      </c>
-      <c r="F27" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" t="b">
-        <v>0</v>
-      </c>
-      <c r="F28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" t="s">
-        <v>91</v>
-      </c>
-      <c r="E29" t="b">
-        <v>0</v>
-      </c>
-      <c r="F29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" t="s">
-        <v>57</v>
-      </c>
-      <c r="C30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" t="b">
-        <v>0</v>
-      </c>
-      <c r="F30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" t="b">
-        <v>0</v>
-      </c>
-      <c r="F31" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" t="b">
-        <v>0</v>
-      </c>
-      <c r="D32" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" t="b">
-        <v>0</v>
-      </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
-        <v>91</v>
-      </c>
-      <c r="E33" t="b">
-        <v>0</v>
-      </c>
-      <c r="F33" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" t="b">
-        <v>0</v>
-      </c>
-      <c r="F34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" t="s">
-        <v>26</v>
-      </c>
-      <c r="B35" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" t="b">
-        <v>0</v>
-      </c>
-      <c r="F35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E36" t="b">
-        <v>0</v>
-      </c>
-      <c r="F36" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
-      <c r="A37" t="s">
-        <v>26</v>
-      </c>
-      <c r="B37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" t="b">
-        <v>0</v>
-      </c>
-      <c r="F37" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" t="s">
-        <v>26</v>
-      </c>
-      <c r="B38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" t="b">
-        <v>0</v>
-      </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
       </c>
       <c r="F38" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" t="b">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="D39" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
       </c>
       <c r="F39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" t="b">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
       </c>
       <c r="F40" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C41" t="b">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
       </c>
       <c r="F41" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" t="b">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
       </c>
       <c r="F42" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
-      </c>
-      <c r="C43" t="b">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="D43" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
       </c>
       <c r="F43" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B44" t="s">
-        <v>71</v>
-      </c>
-      <c r="C44" t="b">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
       </c>
       <c r="F44" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" t="b">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="D45" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
       </c>
       <c r="F45" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
-      </c>
-      <c r="C46" t="b">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
       </c>
       <c r="F46" t="b">
-        <v>1</v>
-      </c>
-      <c r="G46" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B47" t="s">
-        <v>74</v>
-      </c>
-      <c r="C47" t="b">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
       </c>
       <c r="F47" t="b">
-        <v>1</v>
-      </c>
-      <c r="G47" t="s">
-        <v>95</v>
-      </c>
-      <c r="H47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>0</v>
+      </c>
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" t="b">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="D48" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F48" t="b">
         <v>0</v>
       </c>
-      <c r="G48" t="s">
-        <v>96</v>
+      <c r="G48" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
-      </c>
-      <c r="C49" t="b">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="D49" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
       </c>
       <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
-      </c>
-      <c r="C50" t="b">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="D50" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
       </c>
       <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
-      </c>
-      <c r="C51" t="b">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="D51" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
       </c>
       <c r="F51" t="b">
-        <v>1</v>
-      </c>
-      <c r="G51" t="s">
-        <v>97</v>
+        <v>0</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
-      </c>
-      <c r="C52" t="b">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="D52" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
       </c>
       <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" t="b">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="D53" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
       </c>
       <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54" t="b">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="D54" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
       </c>
       <c r="F54" t="b">
-        <v>1</v>
-      </c>
-      <c r="G54" t="s">
-        <v>98</v>
+        <v>0</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B55" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55" t="b">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="D55" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
       </c>
       <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>80</v>
-      </c>
-      <c r="C56" t="b">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="D56" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
       </c>
       <c r="F56" t="b">
-        <v>1</v>
-      </c>
-      <c r="G56" t="s">
-        <v>99</v>
+        <v>0</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
-      </c>
-      <c r="C57" t="b">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D57" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E57" t="b">
         <v>0</v>
       </c>
       <c r="F57" t="b">
-        <v>1</v>
-      </c>
-      <c r="G57" t="s">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>82</v>
-      </c>
-      <c r="C58" t="b">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="D58" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E58" t="b">
         <v>0</v>
       </c>
       <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="G58" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B59" t="s">
-        <v>83</v>
-      </c>
-      <c r="C59" t="b">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="D59" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
       </c>
       <c r="F59" t="b">
-        <v>1</v>
-      </c>
-      <c r="G59" t="s">
-        <v>101</v>
+        <v>0</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
-      </c>
-      <c r="C60" t="b">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="D60" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
       </c>
       <c r="F60" t="b">
-        <v>1</v>
-      </c>
-      <c r="G60" t="s">
-        <v>102</v>
+        <v>0</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
-      </c>
-      <c r="C61" t="b">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="D61" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
       </c>
       <c r="F61" t="b">
-        <v>1</v>
-      </c>
-      <c r="G61" t="s">
-        <v>103</v>
+        <v>0</v>
+      </c>
+      <c r="G61" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B62" t="s">
-        <v>86</v>
-      </c>
-      <c r="C62" t="b">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="D62" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
       </c>
       <c r="F62" t="b">
+        <v>0</v>
+      </c>
+      <c r="G62" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B63" t="s">
-        <v>87</v>
-      </c>
-      <c r="C63" t="b">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="D63" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
       </c>
       <c r="F63" t="b">
+        <v>0</v>
+      </c>
+      <c r="G63" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B64" t="s">
-        <v>73</v>
-      </c>
-      <c r="C64" t="b">
-        <v>1</v>
+        <v>97</v>
       </c>
       <c r="D64" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="E64" t="b">
         <v>0</v>
       </c>
       <c r="F64" t="b">
-        <v>1</v>
-      </c>
-      <c r="G64" t="s">
-        <v>94</v>
+        <v>0</v>
+      </c>
+      <c r="G64" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
-      </c>
-      <c r="C65" t="b">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="D65" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
       </c>
       <c r="F65" t="b">
-        <v>1</v>
-      </c>
-      <c r="G65" t="s">
-        <v>95</v>
-      </c>
-      <c r="H65" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="G65" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>75</v>
-      </c>
-      <c r="C66" t="b">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="D66" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E66" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F66" t="b">
         <v>0</v>
       </c>
-      <c r="G66" t="s">
-        <v>96</v>
+      <c r="G66" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B67" t="s">
-        <v>88</v>
-      </c>
-      <c r="C67" t="b">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D67" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
       </c>
       <c r="F67" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B68" t="s">
-        <v>89</v>
-      </c>
-      <c r="C68" t="b">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="D68" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E68" t="b">
         <v>0</v>
       </c>
       <c r="F68" t="b">
+        <v>0</v>
+      </c>
+      <c r="G68" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s">
-        <v>90</v>
-      </c>
-      <c r="C69" t="b">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D69" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
       </c>
       <c r="F69" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B70" t="s">
-        <v>73</v>
-      </c>
-      <c r="C70" t="b">
-        <v>1</v>
+        <v>103</v>
+      </c>
+      <c r="C70" t="s">
+        <v>128</v>
       </c>
       <c r="D70" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -2262,31 +2442,31 @@
       <c r="F70" t="b">
         <v>1</v>
       </c>
-      <c r="G70" t="s">
-        <v>94</v>
+      <c r="G70" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
-      </c>
-      <c r="C71" t="b">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="C71" t="s">
+        <v>129</v>
       </c>
       <c r="D71" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="E71" t="b">
         <v>0</v>
       </c>
       <c r="F71" t="b">
-        <v>1</v>
-      </c>
-      <c r="G71" t="s">
-        <v>95</v>
+        <v>0</v>
+      </c>
+      <c r="G71" t="b">
+        <v>1</v>
       </c>
       <c r="H71" t="b">
         <v>0</v>
@@ -2294,25 +2474,25 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B72" t="s">
-        <v>75</v>
-      </c>
-      <c r="C72" t="b">
-        <v>1</v>
+        <v>104</v>
+      </c>
+      <c r="C72" t="s">
+        <v>130</v>
       </c>
       <c r="D72" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="E72" t="b">
         <v>1</v>
       </c>
       <c r="F72" t="b">
-        <v>0</v>
-      </c>
-      <c r="G72" t="s">
-        <v>96</v>
+        <v>1</v>
+      </c>
+      <c r="G72" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>